<commit_message>
Expanded with comparision of random strings
Looked at efficiencies of random strings of decimal, hex digits, fixed and mixed case letters, and binary data (equivalent to symmetric encryption keys).
</commit_message>
<xml_diff>
--- a/Password efficiency of word lengths.xlsx
+++ b/Password efficiency of word lengths.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Bits of entropy with:</t>
   </si>
@@ -67,16 +67,46 @@
     <t>2 and 3 char</t>
   </si>
   <si>
+    <t>The clear winner</t>
+  </si>
+  <si>
     <t>2, 3, and 4 char</t>
   </si>
   <si>
     <t>Dicewords</t>
   </si>
   <si>
+    <t>(6^5 words, 32961 characters total)</t>
+  </si>
+  <si>
+    <t>Random strings of characters, for comparison</t>
+  </si>
+  <si>
+    <t>Decimal digits</t>
+  </si>
+  <si>
+    <t>Hex digits</t>
+  </si>
+  <si>
+    <t>(should be exactly 4.0, rounding errors due to use of natural log)</t>
+  </si>
+  <si>
+    <t>Random letters</t>
+  </si>
+  <si>
+    <t>Mixed case letters</t>
+  </si>
+  <si>
+    <t>Binary</t>
+  </si>
+  <si>
+    <t>(same as above, but 8.0)</t>
+  </si>
+  <si>
     <t>source for word counts:  https://www.wordfind.com/scrabble-word-list/</t>
   </si>
   <si>
-    <t>source for Dicewords:  http://world.std.com/~reinhold/diceware.html (6^5 words, 32961 characters total)</t>
+    <t>source for Dicewords:  http://world.std.com/~reinhold/diceware.html</t>
   </si>
 </sst>
 </file>
@@ -137,6 +167,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="31.57"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1"/>
@@ -428,10 +461,13 @@
         <f t="shared" si="6"/>
         <v>3.473179265</v>
       </c>
+      <c r="J9" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1">
         <f>(B3*C3 + B4*C4+B5*C5)/(C3+C4+C5)</f>
@@ -468,7 +504,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1">
         <v>4.239</v>
@@ -500,20 +536,218 @@
         <f t="shared" si="6"/>
         <v>3.043328186</v>
       </c>
+      <c r="J11" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="2"/>
     </row>
     <row r="13">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="2"/>
     </row>
     <row r="14">
-      <c r="B14" s="1" t="s">
-        <v>21</v>
+      <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" ref="D14:D18" si="7">1.44*ln(C14)</f>
+        <v>3.315722534</v>
+      </c>
+      <c r="E14">
+        <f t="shared" ref="E14:E18" si="8">1.44*ln(C14^2)</f>
+        <v>6.631445068</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ref="F14:F18" si="9">1.44*ln(C14^3)</f>
+        <v>9.947167602</v>
+      </c>
+      <c r="G14">
+        <f t="shared" ref="G14:G18" si="10">1.44*ln(C14^4)</f>
+        <v>13.26289014</v>
+      </c>
+      <c r="H14">
+        <f t="shared" ref="H14:H18" si="11">1.44*ln(C14^5)</f>
+        <v>16.57861267</v>
+      </c>
+      <c r="I14">
+        <f t="shared" ref="I14:I18" si="12">D14/(B14)</f>
+        <v>3.315722534</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>16.0</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="7"/>
+        <v>3.99252776</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="8"/>
+        <v>7.98505552</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="9"/>
+        <v>11.97758328</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="10"/>
+        <v>15.97011104</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="11"/>
+        <v>19.9626388</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="12"/>
+        <v>3.99252776</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>26.0</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" si="7"/>
+        <v>4.691659015</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="8"/>
+        <v>9.38331803</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="9"/>
+        <v>14.07497704</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="10"/>
+        <v>18.76663606</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="11"/>
+        <v>23.45829507</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="12"/>
+        <v>4.691659015</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C17" s="1">
+        <v>52.0</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="7"/>
+        <v>5.689790955</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="8"/>
+        <v>11.37958191</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="9"/>
+        <v>17.06937286</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="10"/>
+        <v>22.75916382</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="11"/>
+        <v>28.44895477</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="12"/>
+        <v>5.689790955</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C18" s="1">
+        <v>256.0</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="shared" si="7"/>
+        <v>7.98505552</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="8"/>
+        <v>15.97011104</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="9"/>
+        <v>23.95516656</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="10"/>
+        <v>31.94022208</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="11"/>
+        <v>39.9252776</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="12"/>
+        <v>7.98505552</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>